<commit_message>
update dos arquivos e melhores codigos
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,21 +454,6 @@
           <t>Data</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -481,22 +466,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -509,22 +491,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5,48</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -537,22 +516,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -565,22 +541,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -593,24 +566,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -623,24 +591,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -653,24 +616,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -683,24 +641,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -713,26 +666,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -745,26 +691,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -777,26 +716,19 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>6</v>
-      </c>
-      <c r="G12" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -809,26 +741,19 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>7</v>
-      </c>
-      <c r="G13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -841,27 +766,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>8</v>
-      </c>
-      <c r="G14" t="n">
-        <v>4</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -875,27 +791,18 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>9</v>
-      </c>
-      <c r="G15" t="n">
-        <v>5</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1</v>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -909,27 +816,18 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>10</v>
-      </c>
-      <c r="G16" t="n">
-        <v>6</v>
-      </c>
-      <c r="H16" t="n">
-        <v>2</v>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -943,27 +841,1518 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4,93</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>5,44</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0,037</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4,93</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>5,45</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0,037</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>4,93</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>5,44</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0,037</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>4,93</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>5,44</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0,037</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>5,48</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>0,73</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
         <is>
           <t>21:20</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>11</v>
-      </c>
-      <c r="G17" t="n">
-        <v>7</v>
-      </c>
-      <c r="H17" t="n">
-        <v>3</v>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>4,93</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>5,45</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0,037</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>4,93</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>5,44</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0,037</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>4,93</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>5,44</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0,037</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0,72</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>5,48</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correção e reinstalação de bibliotecas
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,17 +466,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4,93</t>
+          <t>4,91</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -491,17 +491,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -521,12 +521,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,72</t>
+          <t>0,71</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -591,12 +591,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -791,12 +791,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -991,12 +991,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1091,12 +1091,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1266,17 +1266,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1291,17 +1291,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>5,48</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1316,17 +1316,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1391,12 +1391,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,48</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1666,17 +1666,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>4,93</t>
+          <t>5,03</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1691,17 +1691,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,49</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1716,17 +1716,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0,037</t>
+          <t>0,038</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1741,17 +1741,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0,72</t>
+          <t>0,73</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1791,12 +1791,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1966,17 +1966,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1991,17 +1991,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>5,48</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2016,17 +2016,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2041,17 +2041,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2091,12 +2091,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,48</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2350,6 +2350,106 @@
         </is>
       </c>
       <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
         <is>
           <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>

</xml_diff>

<commit_message>
remoção de codigo desnecessário
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -566,17 +566,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4,93</t>
+          <t>4,91</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -591,17 +591,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -621,12 +621,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0,72</t>
+          <t>0,71</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> sábado, 15 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -691,12 +691,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -891,12 +891,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>17:47</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1091,12 +1091,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1191,12 +1191,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1366,17 +1366,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>5,48</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1416,17 +1416,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1441,17 +1441,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1491,12 +1491,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,48</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1766,17 +1766,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>4,93</t>
+          <t>5,03</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>5,45</t>
+          <t>5,49</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1816,17 +1816,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0,037</t>
+          <t>0,038</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1841,17 +1841,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0,72</t>
+          <t>0,73</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1891,12 +1891,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>5,44</t>
+          <t>5,45</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2066,17 +2066,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>5,03</t>
+          <t>4,93</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2091,17 +2091,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>5,48</t>
+          <t>5,44</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2116,17 +2116,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,037</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2141,17 +2141,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0,73</t>
+          <t>0,72</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+          <t xml:space="preserve"> quinta-feira, 13 de abril de 2023 </t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2191,12 +2191,12 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,48</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:32</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2450,6 +2450,106 @@
         </is>
       </c>
       <c r="E81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Dollar</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>5,03</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>5,49</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Iene</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0,038</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Yuan Chinês</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0,73</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
         <is>
           <t xml:space="preserve"> quarta-feira, 5 de abril de 2023 </t>
         </is>

</xml_diff>